<commit_message>
Guardad les dades a llistes (r)
</commit_message>
<xml_diff>
--- a/DocumentacioProjecte/Completion_Table.xlsx
+++ b/DocumentacioProjecte/Completion_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\BNO\DocumentacioProjecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE91E5CE-B8E1-4D69-B1A8-427352F7FB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189A20B-04A3-4E62-B7A1-6ADA20389B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
   <si>
     <t>Distr graus</t>
   </si>
@@ -102,9 +102,6 @@
     <t>C elegnas - sw</t>
   </si>
   <si>
-    <t>FALTA GUARDAD</t>
-  </si>
-  <si>
     <t>C elegans -ba</t>
   </si>
   <si>
@@ -133,6 +130,12 @@
   </si>
   <si>
     <t>Zebrafish larva - ba</t>
+  </si>
+  <si>
+    <t>Tarda</t>
+  </si>
+  <si>
+    <t>TARDA</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,237 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -893,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E986D3-4A1A-4307-8A36-9F77A31AE68A}">
   <dimension ref="B1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,7 +1196,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>16</v>
@@ -972,7 +1205,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>17</v>
@@ -995,13 +1228,13 @@
         <v>16</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>16</v>
@@ -1010,7 +1243,7 @@
         <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>17</v>
@@ -1033,13 +1266,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>16</v>
@@ -1048,7 +1281,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>17</v>
@@ -1065,19 +1298,19 @@
     </row>
     <row r="6" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>16</v>
@@ -1086,7 +1319,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>17</v>
@@ -1106,25 +1339,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>17</v>
@@ -1141,28 +1374,28 @@
     </row>
     <row r="8" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>17</v>
@@ -1179,7 +1412,7 @@
     </row>
     <row r="9" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>16</v>
@@ -1191,7 +1424,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>16</v>
@@ -1200,7 +1433,7 @@
         <v>17</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>17</v>
@@ -1217,7 +1450,7 @@
     </row>
     <row r="10" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>16</v>
@@ -1293,7 +1526,7 @@
     </row>
     <row r="12" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>17</v>
@@ -1331,7 +1564,7 @@
     </row>
     <row r="13" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>16</v>
@@ -1369,7 +1602,7 @@
     </row>
     <row r="14" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>16</v>
@@ -1445,7 +1678,7 @@
     </row>
     <row r="16" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>17</v>
@@ -1483,7 +1716,7 @@
     </row>
     <row r="17" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>17</v>
@@ -1521,7 +1754,7 @@
     </row>
     <row r="18" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>17</v>
@@ -1610,7 +1843,7 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
@@ -1631,48 +1864,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M6 C15:M19 D7:M14">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C14">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C10">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="TARDA">
+      <formula>NOT(ISERROR(SEARCH("TARDA",G8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:M19">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TARDA">
+      <formula>NOT(ISERROR(SEARCH("TARDA",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Afegir contingut i guardar dades (r)
</commit_message>
<xml_diff>
--- a/DocumentacioProjecte/Completion_Table.xlsx
+++ b/DocumentacioProjecte/Completion_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\BNO\DocumentacioProjecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189A20B-04A3-4E62-B7A1-6ADA20389B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293655CA-23AC-413E-BED7-5878439C0CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
+    <workbookView xWindow="3432" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
   </bookViews>
   <sheets>
     <sheet name="Full1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -464,236 +464,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1127,7 +897,7 @@
   <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1456,13 +1226,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>16</v>
@@ -1471,7 +1241,7 @@
         <v>17</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>17</v>
@@ -1500,7 +1270,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>16</v>
@@ -1509,7 +1279,7 @@
         <v>17</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>17</v>
@@ -1864,52 +1634,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M6 C15:M19 D7:M14">
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C14">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:C10">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="SI">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="TARDA">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="TARDA">
       <formula>NOT(ISERROR(SEARCH("TARDA",G8)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Afegir contingut taula i r
</commit_message>
<xml_diff>
--- a/DocumentacioProjecte/Completion_Table.xlsx
+++ b/DocumentacioProjecte/Completion_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\BNO\DocumentacioProjecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293655CA-23AC-413E-BED7-5878439C0CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167755ED-84A4-41C7-8F76-880C3D3CB527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3432" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="33">
   <si>
     <t>Distr graus</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Tarda</t>
-  </si>
-  <si>
-    <t>TARDA</t>
   </si>
 </sst>
 </file>
@@ -896,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E986D3-4A1A-4307-8A36-9F77A31AE68A}">
   <dimension ref="B1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,25 +1106,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>17</v>
@@ -1147,25 +1144,25 @@
         <v>27</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>17</v>
@@ -1299,7 +1296,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>16</v>
@@ -1308,16 +1305,16 @@
         <v>16</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>17</v>
@@ -1346,7 +1343,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>16</v>
@@ -1355,7 +1352,7 @@
         <v>17</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>17</v>
@@ -1384,7 +1381,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>16</v>
@@ -1393,7 +1390,7 @@
         <v>17</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
R: Completa ratoli, afegir Community detection i Cliques. Apuntar tot aixo al excel
</commit_message>
<xml_diff>
--- a/DocumentacioProjecte/Completion_Table.xlsx
+++ b/DocumentacioProjecte/Completion_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\BNO\DocumentacioProjecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167755ED-84A4-41C7-8F76-880C3D3CB527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F1FDD5-08D4-4CF3-A994-E1AC4A27E5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3432" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
   </bookViews>
   <sheets>
     <sheet name="Full1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
   <si>
     <t>Distr graus</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Tarda</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -893,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E986D3-4A1A-4307-8A36-9F77A31AE68A}">
   <dimension ref="B1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,13 +972,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>17</v>
@@ -1007,13 +1010,13 @@
         <v>16</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>17</v>
@@ -1045,13 +1048,13 @@
         <v>16</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>17</v>
@@ -1083,13 +1086,13 @@
         <v>16</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>17</v>
@@ -1121,13 +1124,13 @@
         <v>16</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>17</v>
@@ -1159,13 +1162,13 @@
         <v>16</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>17</v>
@@ -1197,13 +1200,13 @@
         <v>16</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="K9" s="11" t="s">
         <v>17</v>
@@ -1235,13 +1238,13 @@
         <v>16</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>17</v>
@@ -1273,13 +1276,13 @@
         <v>16</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>17</v>
@@ -1317,7 +1320,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>17</v>
@@ -1337,7 +1340,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>16</v>
@@ -1349,13 +1352,13 @@
         <v>16</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>17</v>
@@ -1387,13 +1390,13 @@
         <v>16</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>17</v>
@@ -1562,25 +1565,25 @@
         <v>5</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J19" s="12" t="s">
         <v>17</v>
@@ -1643,7 +1646,7 @@
       <formula>NOT(ISERROR(SEARCH("no",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:M6 C15:M19 D7:M14">
+  <conditionalFormatting sqref="C15:M19 C3:M6 D7:M14">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corregir errors de r, afegir un par de numero de Nodes
</commit_message>
<xml_diff>
--- a/DocumentacioProjecte/Completion_Table.xlsx
+++ b/DocumentacioProjecte/Completion_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\BNO\DocumentacioProjecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F1FDD5-08D4-4CF3-A994-E1AC4A27E5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14F2F68-224F-4819-B69A-F29D4FEA6904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
   </bookViews>
@@ -897,7 +897,7 @@
   <dimension ref="B1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -981,7 +981,7 @@
         <v>16</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>17</v>
@@ -1019,7 +1019,7 @@
         <v>16</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Modificacions R i Excel (mirar desc)
Ordenat tot el codi de r, dividir les parts en diferents archius .r
Completat al 100% C_Elegans i totes les seves xarxes aleatòries. Afegit a l'Excel.
Completat codi Fly Optic i totes les seves xarxes aleatòries , falta revisar error.
Completat codi Ratolí NO les xarxes aleatòries, falta revisar erros.
Ordenar L'Excel i afegir la columna de nNodes.
</commit_message>
<xml_diff>
--- a/DocumentacioProjecte/Completion_Table.xlsx
+++ b/DocumentacioProjecte/Completion_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\OneDrive\Escritorio\BNO\DocumentacioProjecte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14F2F68-224F-4819-B69A-F29D4FEA6904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0599A508-57CC-4F81-ADFD-00B8E722A3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4984B98C-4B75-4CBF-8018-A323BE46E503}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="35">
   <si>
     <t>Distr graus</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">Zebrafish larva </t>
   </si>
   <si>
-    <t>Mouse</t>
-  </si>
-  <si>
     <t>Cens de triades</t>
   </si>
   <si>
@@ -135,7 +132,13 @@
     <t>Tarda</t>
   </si>
   <si>
-    <t>no</t>
+    <t>Mouse-Meso</t>
+  </si>
+  <si>
+    <t>nEdges</t>
+  </si>
+  <si>
+    <t>nNodes</t>
   </si>
 </sst>
 </file>
@@ -894,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E986D3-4A1A-4307-8A36-9F77A31AE68A}">
-  <dimension ref="B1:M31"/>
+  <dimension ref="B1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,725 +913,817 @@
     <col min="6" max="6" width="15.77734375" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="9" width="18.77734375" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="10" max="12" width="17.77734375" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="N2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="O2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="C10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="C14" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L14" s="11"/>
       <c r="M14" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="14"/>
       <c r="C28" s="11"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="14"/>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="14"/>
       <c r="C30" s="11"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="14"/>
       <c r="C31" s="11"/>
     </row>
@@ -1646,7 +1741,7 @@
       <formula>NOT(ISERROR(SEARCH("no",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:M19 C3:M6 D7:M14">
+  <conditionalFormatting sqref="C15:O19 C3:O6 D7:O14 K6:K19">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C3)))</formula>
     </cfRule>
@@ -1670,7 +1765,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C10">
+  <conditionalFormatting sqref="C7:O10">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="SI">
       <formula>NOT(ISERROR(SEARCH("SI",C7)))</formula>
     </cfRule>
@@ -1683,7 +1778,7 @@
       <formula>NOT(ISERROR(SEARCH("TARDA",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:M19">
+  <conditionalFormatting sqref="C3:O19">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TARDA">
       <formula>NOT(ISERROR(SEARCH("TARDA",C3)))</formula>
     </cfRule>

</xml_diff>